<commit_message>
modified:   addhost_v2/addhosts.py 	modified:   addhost_v2/addhostslib/argument_manager.py 	modified:   addhost_v2/addhostslib/destination_host_file.py 	modified:   addhost_v2/addhostslib/excel_host_file.py 	deleted:    addhost_v2/addhostslib/log.py 	addhost_v2/addhosts.bat 	addhost_v2/addhostslib/commonlog.py 	addhost_v2/stat_lines.py
</commit_message>
<xml_diff>
--- a/addhost_v2/file/主机列表.xlsx
+++ b/addhost_v2/file/主机列表.xlsx
@@ -14,33 +14,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>123.57.56.121</t>
   </si>
   <si>
-    <t>webServer</t>
-  </si>
-  <si>
     <t>alias</t>
   </si>
   <si>
-    <t>123.57.56.120</t>
-  </si>
-  <si>
-    <t>MDSServer</t>
-  </si>
-  <si>
-    <t>alias2</t>
-  </si>
-  <si>
-    <t>123.57.56.122</t>
-  </si>
-  <si>
-    <t>DBServer</t>
-  </si>
-  <si>
-    <t>alisa3</t>
+    <t>abc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>123.57.56.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>liujiashuai</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MARS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -400,49 +395,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="B2:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="12.375" customWidth="1"/>
-    <col min="2" max="2" width="10.75" customWidth="1"/>
+    <col min="2" max="2" width="12.375" customWidth="1"/>
+    <col min="3" max="3" width="10.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>